<commit_message>
EBEGU-1199 * Total mutierte WizardSteps korrigiert * Div. Visual Anpassungen/Verbesserungen Excel * Div. Spalten entfernt gemäss Ticket * Riehefolge die Spalten angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchZeitraum.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchZeitraum.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\dev\ebegu\ebegu-server\src\main\resources\reporting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24465" windowHeight="13575"/>
+    <workbookView xWindow="-15" yWindow="2895" windowWidth="24465" windowHeight="13575"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
-    <sheet name="Data" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatapivotabelleData">Data!$A$1:$AF$2</definedName>
+    <definedName name="DatapivotabelleData">Data!$A$1:$AB$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <pivotCaches>
     <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>Institution</t>
   </si>
@@ -58,9 +63,6 @@
     <t>AnzahlMutationBetreuung</t>
   </si>
   <si>
-    <t>AnzahlMutationDokumente</t>
-  </si>
-  <si>
     <t>AnzahlMutationEV</t>
   </si>
   <si>
@@ -73,12 +75,6 @@
     <t>AnzahlMutationFinanzielleSituation</t>
   </si>
   <si>
-    <t>AnzahlMutationFreigabe</t>
-  </si>
-  <si>
-    <t>AnzahlMutationGesuchErstellen</t>
-  </si>
-  <si>
     <t>AnzahlMutationGesuchsteller</t>
   </si>
   <si>
@@ -88,9 +84,6 @@
     <t>AnzahlMutationUmzug</t>
   </si>
   <si>
-    <t>AnzahlMutationVerfuegen</t>
-  </si>
-  <si>
     <t>AnzahlMahnungen</t>
   </si>
   <si>
@@ -145,9 +138,6 @@
     <t>{anzahlMutationBetreuung}</t>
   </si>
   <si>
-    <t>{anzahlMutationDokumente}</t>
-  </si>
-  <si>
     <t>{anzahlMutationEV}</t>
   </si>
   <si>
@@ -160,12 +150,6 @@
     <t>{anzahlMutationFinanzielleSituation}</t>
   </si>
   <si>
-    <t>{anzahlMutationFreigabe}</t>
-  </si>
-  <si>
-    <t>{anzahlMutationGesuchErstellen}</t>
-  </si>
-  <si>
     <t>{anzahlMutationGesuchsteller}</t>
   </si>
   <si>
@@ -175,9 +159,6 @@
     <t>{anzahlMutationUmzug}</t>
   </si>
   <si>
-    <t>{anzahlMutationVerfuegen}</t>
-  </si>
-  <si>
     <t>{anzahlMahnungen}</t>
   </si>
   <si>
@@ -235,9 +216,6 @@
     <t>Betreuung</t>
   </si>
   <si>
-    <t>Dokumente</t>
-  </si>
-  <si>
     <t>Einkommensverschlechterungen</t>
   </si>
   <si>
@@ -250,12 +228,6 @@
     <t>Finanzielle Situation</t>
   </si>
   <si>
-    <t>Freigabe</t>
-  </si>
-  <si>
-    <t>Gesuch Erstellen</t>
-  </si>
-  <si>
     <t>Gesuchsteller</t>
   </si>
   <si>
@@ -265,9 +237,6 @@
     <t>Umzug</t>
   </si>
   <si>
-    <t>Verfuegen</t>
-  </si>
-  <si>
     <t>Verfügungen</t>
   </si>
   <si>
@@ -307,9 +276,6 @@
     <t>{gesuchLaufNr}</t>
   </si>
   <si>
-    <t>(Alle)</t>
-  </si>
-  <si>
     <t>AnzahlSteueramtAusgeloest</t>
   </si>
   <si>
@@ -332,13 +298,16 @@
   </si>
   <si>
     <t>Ausgestellt</t>
+  </si>
+  <si>
+    <t>(All)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,14 +324,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,8 +350,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -466,64 +441,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Akzent1" xfId="1" builtinId="30"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="104">
+  <dxfs count="236">
     <dxf>
       <border>
         <left style="thin">
@@ -942,6 +1010,930 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1380,11 +2372,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42920.540745949074" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42929.544201504628" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="DatapivotabelleData"/>
   </cacheSource>
-  <cacheFields count="34">
+  <cacheFields count="30">
     <cacheField name="BGNummer" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -1424,9 +2416,6 @@
     <cacheField name="AnzahlMutationBetreuung" numFmtId="0">
       <sharedItems/>
     </cacheField>
-    <cacheField name="AnzahlMutationDokumente" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
     <cacheField name="AnzahlMutationEV" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -1439,12 +2428,6 @@
     <cacheField name="AnzahlMutationFinanzielleSituation" numFmtId="0">
       <sharedItems/>
     </cacheField>
-    <cacheField name="AnzahlMutationFreigabe" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="AnzahlMutationGesuchErstellen" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
     <cacheField name="AnzahlMutationGesuchsteller" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -1452,9 +2435,6 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="AnzahlMutationUmzug" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="AnzahlMutationVerfuegen" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="AnzahlMahnungen" numFmtId="0">
@@ -1512,17 +2492,13 @@
     <s v="{anzahlMutationPapier}"/>
     <s v="{anzahlMutationAbwesenheit}"/>
     <s v="{anzahlMutationBetreuung}"/>
-    <s v="{anzahlMutationDokumente}"/>
     <s v="{anzahlMutationEV}"/>
     <s v="{anzahlMutationEwerbspensum}"/>
     <s v="{anzahlMutationFamilienSitutation}"/>
     <s v="{anzahlMutationFinanzielleSituation}"/>
-    <s v="{anzahlMutationFreigabe}"/>
-    <s v="{anzahlMutationGesuchErstellen}"/>
     <s v="{anzahlMutationGesuchsteller}"/>
     <s v="{anzahlMutationKinder}"/>
     <s v="{anzahlMutationUmzug}"/>
-    <s v="{anzahlMutationVerfuegen}"/>
     <s v="{anzahlMahnungen}"/>
     <s v="{anzahlSteueramtAusgeloest}"/>
     <s v="{anzahlSteueramtGeprueft}"/>
@@ -1538,9 +2514,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="B4:AF7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="34">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="B4:AB7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="30">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
       <items count="1">
@@ -1558,10 +2534,6 @@
       </items>
     </pivotField>
     <pivotField compact="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
@@ -1603,7 +2575,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="29">
+  <colItems count="25">
     <i>
       <x/>
     </i>
@@ -1679,55 +2651,39 @@
     <i i="24">
       <x v="24"/>
     </i>
-    <i i="25">
-      <x v="25"/>
-    </i>
-    <i i="26">
-      <x v="26"/>
-    </i>
-    <i i="27">
-      <x v="27"/>
-    </i>
-    <i i="28">
-      <x v="28"/>
-    </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="3" hier="-1"/>
   </pageFields>
-  <dataFields count="29">
-    <dataField name="Total" fld="33" baseField="0" baseItem="0"/>
+  <dataFields count="25">
+    <dataField name="Total" fld="29" baseField="0" baseItem="0"/>
     <dataField name="Online" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Papier" fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Total " fld="32" baseField="1" baseItem="0"/>
+    <dataField name="Total " fld="28" baseField="1" baseItem="0"/>
     <dataField name="Online " fld="7" baseField="1" baseItem="0"/>
     <dataField name="Papier " fld="8" baseField="1" baseItem="0"/>
+    <dataField name="Familien Situtation" fld="13" baseField="0" baseItem="0"/>
+    <dataField name="Gesuchsteller" fld="15" baseField="0" baseItem="0"/>
+    <dataField name="Umzug" fld="17" baseField="0" baseItem="0"/>
+    <dataField name="Kinder" fld="16" baseField="0" baseItem="0"/>
+    <dataField name="Betreuung" fld="10" baseField="0" baseItem="0"/>
     <dataField name="Abwesenheit" fld="9" baseField="0" baseItem="0"/>
-    <dataField name="Betreuung" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Dokumente" fld="11" baseField="0" baseItem="0"/>
-    <dataField name="Einkommensverschlechterungen" fld="12" baseField="0" baseItem="0"/>
-    <dataField name="Ewerbspensum" fld="13" baseField="0" baseItem="0"/>
-    <dataField name="Familien Situtation" fld="14" baseField="0" baseItem="0"/>
-    <dataField name="Finanzielle Situation" fld="15" baseField="0" baseItem="0"/>
-    <dataField name="Freigabe" fld="16" baseField="0" baseItem="0"/>
-    <dataField name="Gesuch Erstellen" fld="17" baseField="0" baseItem="0"/>
-    <dataField name="Gesuchsteller" fld="18" baseField="0" baseItem="0"/>
-    <dataField name="Kinder" fld="19" baseField="0" baseItem="0"/>
-    <dataField name="Umzug" fld="20" baseField="0" baseItem="0"/>
-    <dataField name="Verfuegen" fld="21" baseField="0" baseItem="0"/>
-    <dataField name="Ausgestellt" fld="22" baseField="0" baseItem="0"/>
-    <dataField name="Prüfungen ausgelöst" fld="23" baseField="0" baseItem="0"/>
-    <dataField name="Geprüft" fld="24" baseField="0" baseItem="0"/>
-    <dataField name="Ausgelöste" fld="25" baseField="0" baseItem="0"/>
-    <dataField name="Ausgestellte" fld="26" baseField="0" baseItem="0"/>
-    <dataField name="Normale" fld="27" baseField="0" baseItem="0"/>
-    <dataField name="Max Einkommen" fld="28" baseField="0" baseItem="0"/>
-    <dataField name="Kein Pensum" fld="29" baseField="0" baseItem="0"/>
-    <dataField name="Zuschlag zum Pensum" fld="30" baseField="0" baseItem="0"/>
-    <dataField name="Nichteintreten" fld="31" baseField="0" baseItem="0"/>
+    <dataField name="Ewerbspensum" fld="12" baseField="0" baseItem="0"/>
+    <dataField name="Finanzielle Situation" fld="14" baseField="0" baseItem="0"/>
+    <dataField name="Einkommensverschlechterungen" fld="11" baseField="0" baseItem="0"/>
+    <dataField name="Ausgestellt" fld="18" baseField="0" baseItem="0"/>
+    <dataField name="Prüfungen ausgelöst" fld="19" baseField="0" baseItem="0"/>
+    <dataField name="Geprüft" fld="20" baseField="0" baseItem="0"/>
+    <dataField name="Ausgelöste" fld="21" baseField="0" baseItem="0"/>
+    <dataField name="Ausgestellte" fld="22" baseField="0" baseItem="0"/>
+    <dataField name="Normale" fld="23" baseField="0" baseItem="0"/>
+    <dataField name="Max Einkommen" fld="24" baseField="0" baseItem="0"/>
+    <dataField name="Kein Pensum" fld="25" baseField="0" baseItem="0"/>
+    <dataField name="Zuschlag zum Pensum" fld="26" baseField="0" baseItem="0"/>
+    <dataField name="Nichteintreten" fld="27" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="52">
-    <format dxfId="103">
+  <formats count="118">
+    <format dxfId="235">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -1738,7 +2694,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="234">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -1749,7 +2705,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="233">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -1760,7 +2716,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="232">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -1771,10 +2727,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="231">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="16" selected="0">
+          <reference field="4294967294" count="12" selected="0">
             <x v="3"/>
             <x v="4"/>
             <x v="5"/>
@@ -1787,18 +2743,14 @@
             <x v="12"/>
             <x v="13"/>
             <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="16">
+    <format dxfId="230">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12">
             <x v="3"/>
             <x v="4"/>
             <x v="5"/>
@@ -1811,15 +2763,11 @@
             <x v="12"/>
             <x v="13"/>
             <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="229">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1828,7 +2776,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="228">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1838,7 +2786,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="227">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1849,7 +2797,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="226">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1858,7 +2806,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="225">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1868,7 +2816,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="224">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1879,7 +2827,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="223">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -1890,7 +2838,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="222">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -1901,10 +2849,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="221">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="16" selected="0">
+          <reference field="4294967294" count="12" selected="0">
             <x v="3"/>
             <x v="4"/>
             <x v="5"/>
@@ -1917,18 +2865,14 @@
             <x v="12"/>
             <x v="13"/>
             <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="16">
+    <format dxfId="220">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12">
             <x v="3"/>
             <x v="4"/>
             <x v="5"/>
@@ -1941,34 +2885,30 @@
             <x v="12"/>
             <x v="13"/>
             <x v="14"/>
-            <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
-            <x v="18"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="219">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="86">
+    <format dxfId="218">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="217">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="216">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="215">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="214">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -1976,10 +2916,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="27">
+    <format dxfId="213">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="23">
             <x v="0"/>
             <x v="1"/>
             <x v="2"/>
@@ -1996,25 +2936,21 @@
             <x v="13"/>
             <x v="14"/>
             <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
             <x v="18"/>
             <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
             <x v="22"/>
             <x v="23"/>
             <x v="24"/>
-            <x v="25"/>
-            <x v="26"/>
-            <x v="27"/>
-            <x v="28"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="27">
+    <format dxfId="212">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="23">
             <x v="0"/>
             <x v="1"/>
             <x v="2"/>
@@ -2031,35 +2967,31 @@
             <x v="13"/>
             <x v="14"/>
             <x v="15"/>
-            <x v="16"/>
-            <x v="17"/>
             <x v="18"/>
             <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
             <x v="22"/>
             <x v="23"/>
             <x v="24"/>
-            <x v="25"/>
-            <x v="26"/>
-            <x v="27"/>
-            <x v="28"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="211">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="210">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="209">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="208">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2067,14 +2999,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="207">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="206">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2082,14 +3014,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="205">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="204">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2097,14 +3029,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="203">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="202">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2112,14 +3044,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="201">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="200">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2127,14 +3059,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="199">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="198">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2142,83 +3074,582 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="197">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="196">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="195">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="194">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="193">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="192">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="191">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="190">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="189">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="188">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="187">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="186">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="185">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="184">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="183">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="182">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="181">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="A1:B1" fieldPosition="0"/>
+    </format>
+    <format dxfId="180">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="179">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="178">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="177">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12" selected="0">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="176">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12" selected="0">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="175">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="174">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="173">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="172">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="171">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="170">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="169">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="168">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="167">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="166">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="165">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="164">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="163">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="162">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="161">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="160">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="159">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="158">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="A1:B1" fieldPosition="0"/>
+    </format>
+    <format dxfId="157">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="156">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12" selected="0">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="155">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1:N1" fieldPosition="0"/>
+    </format>
+    <format dxfId="154">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="153">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="152">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="O1" fieldPosition="0"/>
+    </format>
+    <format dxfId="151">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="15"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="150">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="149">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="R1" fieldPosition="0"/>
+    </format>
+    <format dxfId="148">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="147">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="P1:Q1" fieldPosition="0"/>
+    </format>
+    <format dxfId="146">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="16"/>
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="145">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
+    </format>
+    <format dxfId="144">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="143">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12" selected="0">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="142">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1:N1" fieldPosition="0"/>
+    </format>
+    <format dxfId="141">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="12">
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="140">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="139">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="138">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="137">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="136">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="135">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="16"/>
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="134">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="P1:Q1" fieldPosition="0"/>
+    </format>
+    <format dxfId="133">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2">
+            <x v="16"/>
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="132">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6" selected="0">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="131">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
+    </format>
+    <format dxfId="130">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="129">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6" selected="0">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="128">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
+    </format>
+    <format dxfId="127">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="126">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="19"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="125">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="20"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="124">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="123">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2227,12 +3658,63 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="122">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
             <x v="21"/>
           </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="121">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="120">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="6">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="119">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="6" selected="0">
+            <x v="19"/>
+            <x v="20"/>
+            <x v="21"/>
+            <x v="22"/>
+            <x v="23"/>
+            <x v="24"/>
+          </reference>
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="118">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
@@ -2289,7 +3771,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2341,7 +3823,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2535,807 +4017,780 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AF29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AB29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" customWidth="1"/>
-    <col min="21" max="21" width="6.85546875" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" customWidth="1"/>
-    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>93</v>
+      <c r="C2" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="3" spans="2:32" s="1" customFormat="1">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="15" t="s">
+    <row r="3" spans="2:28" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" s="22"/>
+      <c r="V3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="22"/>
+    </row>
+    <row r="4" spans="2:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+    </row>
+    <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="X3" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="19"/>
+      <c r="Q5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="R5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="T5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="W5" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="X5" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y5" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB5" s="18" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="4" spans="2:32">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
     </row>
-    <row r="5" spans="2:32">
-      <c r="B5" s="8" t="s">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="11">
         <v>0</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y5" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z5" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA5" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB5" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC5" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD5" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE5" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF5" s="10" t="s">
-        <v>89</v>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0</v>
+      </c>
+      <c r="S7" s="11">
+        <v>0</v>
+      </c>
+      <c r="T7" s="10">
+        <v>0</v>
+      </c>
+      <c r="U7" s="10">
+        <v>0</v>
+      </c>
+      <c r="V7" s="11">
+        <v>0</v>
+      </c>
+      <c r="W7" s="17">
+        <v>0</v>
+      </c>
+      <c r="X7" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="17">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:32">
-      <c r="B6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
     </row>
-    <row r="7" spans="2:32">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>0</v>
-      </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
-      <c r="T7" s="3">
-        <v>0</v>
-      </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3">
-        <v>0</v>
-      </c>
-      <c r="X7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3">
-        <v>0</v>
-      </c>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
     </row>
-    <row r="10" spans="2:32">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
     </row>
-    <row r="11" spans="2:32">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
     </row>
-    <row r="12" spans="2:32">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="AA13" s="5"/>
     </row>
-    <row r="13" spans="2:32">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="AA13" s="11"/>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
     </row>
-    <row r="14" spans="2:32">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
     </row>
-    <row r="15" spans="2:32">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
     </row>
-    <row r="16" spans="2:32">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
     </row>
-    <row r="17" spans="2:21">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
     </row>
-    <row r="18" spans="2:21">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
     </row>
-    <row r="19" spans="2:21">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
     </row>
-    <row r="20" spans="2:21">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
     </row>
-    <row r="21" spans="2:21">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
     </row>
-    <row r="22" spans="2:21">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
     </row>
-    <row r="23" spans="2:21">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
     </row>
-    <row r="24" spans="2:21">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
     </row>
-    <row r="25" spans="2:21">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
     </row>
-    <row r="26" spans="2:21">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
     </row>
-    <row r="27" spans="2:21">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
     </row>
-    <row r="28" spans="2:21">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-    </row>
-    <row r="29" spans="2:21">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="W3:AB3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:V3"/>
-    <mergeCell ref="AA3:AF3"/>
-    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="G3:R3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3343,14 +4798,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3:Z3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -3363,31 +4818,27 @@
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="37.140625" customWidth="1"/>
-    <col min="24" max="24" width="37" customWidth="1"/>
-    <col min="25" max="25" width="42.7109375" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.140625" customWidth="1"/>
+    <col min="20" max="20" width="37" customWidth="1"/>
+    <col min="21" max="21" width="42.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3401,7 +4852,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -3446,22 +4897,22 @@
         <v>17</v>
       </c>
       <c r="T1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>96</v>
       </c>
       <c r="Z1" t="s">
         <v>22</v>
@@ -3472,118 +4923,94 @@
       <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" t="s">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:33">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>41</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
         <v>42</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>44</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>46</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Z2" t="s">
         <v>47</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>48</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>49</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AC2" t="s">
         <v>50</v>
-      </c>
-      <c r="X2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>